<commit_message>
Update according to 11.12 changes
</commit_message>
<xml_diff>
--- a/examples/примеры.xlsx
+++ b/examples/примеры.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanyakovenko/Documents/Моя Схемота/БО/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanyakovenko/Documents/Моя Схемота/БО/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{171917D1-6A85-D14C-B7A6-8528A23CB4F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F1C16C-419E-A34A-9572-FDD87AA0148D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16480" xr2:uid="{BF272BA3-E648-DD4C-99B8-5F87B9EA626A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>RR = 0</t>
   </si>
@@ -115,13 +115,28 @@
   </si>
   <si>
     <t>k = 3 b3 = 1 - 1 = 0</t>
+  </si>
+  <si>
+    <t>RB0</t>
+  </si>
+  <si>
+    <t>RB1</t>
+  </si>
+  <si>
+    <t>RB2</t>
+  </si>
+  <si>
+    <t>RB3</t>
+  </si>
+  <si>
+    <t>ZF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +148,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -343,22 +365,10 @@
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -373,9 +383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -386,6 +393,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,17 +723,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A46FDC0-C2F7-6D4F-8BE0-346CDF963741}">
-  <dimension ref="A1:V65"/>
+  <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74:G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="2.5" customWidth="1"/>
+    <col min="3" max="6" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="2.5" customWidth="1"/>
     <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,31 +745,31 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="18">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="20" t="s">
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>0</v>
       </c>
     </row>
@@ -753,139 +777,139 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="21"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="14">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="22" t="s">
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="14">
-        <v>0</v>
-      </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="20" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C7" s="15">
-        <v>0</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="21" t="s">
+      <c r="C7" s="11">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C8" s="14">
-        <v>0</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="22" t="s">
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -893,48 +917,48 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="20"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="14">
-        <v>0</v>
-      </c>
-      <c r="D10" s="13">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="22" t="s">
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -942,75 +966,75 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="20" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="10">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="C12" s="15">
-        <v>1</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="22" t="s">
+      <c r="A12" s="5"/>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1018,31 +1042,31 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="14">
-        <v>0</v>
-      </c>
-      <c r="D18" s="13">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-      <c r="J18" s="14">
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="10">
         <v>0</v>
       </c>
       <c r="K18" t="s">
@@ -1050,95 +1074,95 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0</v>
-      </c>
-      <c r="J19" s="6">
-        <v>0</v>
-      </c>
-      <c r="K19" s="20" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="10">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
-      <c r="C20" s="15">
-        <v>1</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0</v>
-      </c>
-      <c r="J20" s="6">
-        <v>0</v>
-      </c>
-      <c r="K20" s="21" t="s">
+      <c r="C20" s="11">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
-      <c r="C21" s="14">
-        <v>1</v>
-      </c>
-      <c r="D21" s="13">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" s="3">
-        <v>1</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0</v>
-      </c>
-      <c r="J21" s="6">
-        <v>0</v>
-      </c>
-      <c r="K21" s="21" t="s">
+      <c r="C21" s="10">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1147,217 +1171,217 @@
         <v>11</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="20"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="16"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="14">
-        <v>1</v>
-      </c>
-      <c r="D23" s="13">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0</v>
-      </c>
-      <c r="G23" s="3">
-        <v>1</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-      <c r="J23" s="6">
-        <v>0</v>
-      </c>
-      <c r="K23" s="22" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="17">
-        <v>0</v>
-      </c>
-      <c r="D24" s="16">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
-        <v>1</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5">
-        <v>0</v>
-      </c>
-      <c r="J24" s="23">
-        <v>0</v>
-      </c>
-      <c r="K24" s="21" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="13">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="19">
+        <v>0</v>
+      </c>
+      <c r="K24" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
-      <c r="C25" s="15">
-        <v>0</v>
-      </c>
-      <c r="D25" s="13">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1</v>
-      </c>
-      <c r="H25" s="3">
-        <v>1</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0</v>
-      </c>
-      <c r="J25" s="6">
-        <v>0</v>
-      </c>
-      <c r="K25" s="21" t="s">
+      <c r="C25" s="11">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="14">
-        <v>0</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="3">
-        <v>1</v>
-      </c>
-      <c r="J26" s="6">
-        <v>0</v>
-      </c>
-      <c r="K26" s="21" t="s">
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="14">
-        <v>1</v>
-      </c>
-      <c r="D27" s="13">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1</v>
-      </c>
-      <c r="F27" s="3">
-        <v>1</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
-        <v>0</v>
-      </c>
-      <c r="J27" s="6">
-        <v>0</v>
-      </c>
-      <c r="K27" s="20" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="10">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0</v>
+      </c>
+      <c r="K27" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
-      <c r="C28" s="15">
-        <v>1</v>
-      </c>
-      <c r="D28" s="13">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3">
-        <v>1</v>
-      </c>
-      <c r="I28" s="3">
-        <v>1</v>
-      </c>
-      <c r="J28" s="6">
-        <v>0</v>
-      </c>
-      <c r="K28" s="22" t="s">
+      <c r="C28" s="11">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1365,28 +1389,28 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="O33" s="14">
-        <v>0</v>
-      </c>
-      <c r="P33" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="3">
-        <v>1</v>
-      </c>
-      <c r="R33" s="3">
-        <v>0</v>
-      </c>
-      <c r="S33" s="3">
-        <v>1</v>
-      </c>
-      <c r="T33" s="3">
-        <v>1</v>
-      </c>
-      <c r="U33" s="3">
-        <v>0</v>
-      </c>
-      <c r="V33" s="6">
+      <c r="O33" s="10">
+        <v>0</v>
+      </c>
+      <c r="P33" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>1</v>
+      </c>
+      <c r="R33" s="2">
+        <v>0</v>
+      </c>
+      <c r="S33" s="2">
+        <v>1</v>
+      </c>
+      <c r="T33" s="2">
+        <v>1</v>
+      </c>
+      <c r="U33" s="2">
+        <v>0</v>
+      </c>
+      <c r="V33" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1418,28 +1442,28 @@
       <c r="K34" t="s">
         <v>0</v>
       </c>
-      <c r="O34" s="17">
-        <v>0</v>
-      </c>
-      <c r="P34" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="5">
-        <v>0</v>
-      </c>
-      <c r="R34" s="5">
-        <v>1</v>
-      </c>
-      <c r="S34" s="5">
-        <v>0</v>
-      </c>
-      <c r="T34" s="5">
-        <v>0</v>
-      </c>
-      <c r="U34" s="5">
-        <v>0</v>
-      </c>
-      <c r="V34" s="23">
+      <c r="O34" s="13">
+        <v>0</v>
+      </c>
+      <c r="P34" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>0</v>
+      </c>
+      <c r="R34" s="3">
+        <v>1</v>
+      </c>
+      <c r="S34" s="3">
+        <v>0</v>
+      </c>
+      <c r="T34" s="3">
+        <v>0</v>
+      </c>
+      <c r="U34" s="3">
+        <v>0</v>
+      </c>
+      <c r="V34" s="19">
         <v>0</v>
       </c>
     </row>
@@ -1471,7 +1495,7 @@
       <c r="J35">
         <v>0</v>
       </c>
-      <c r="K35" s="19" t="s">
+      <c r="K35" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1585,7 +1609,7 @@
       <c r="J38">
         <v>0</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K38" s="15" t="s">
         <v>5</v>
       </c>
       <c r="O38">
@@ -1638,7 +1662,7 @@
       <c r="J39">
         <v>0</v>
       </c>
-      <c r="K39" s="25" t="s">
+      <c r="K39" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1667,7 +1691,7 @@
       <c r="J40">
         <v>0</v>
       </c>
-      <c r="K40" s="25" t="s">
+      <c r="K40" s="20" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1699,7 +1723,7 @@
       <c r="J41">
         <v>0</v>
       </c>
-      <c r="K41" s="19" t="s">
+      <c r="K41" s="15" t="s">
         <v>15</v>
       </c>
       <c r="O41" t="s">
@@ -1731,7 +1755,7 @@
       <c r="J42">
         <v>0</v>
       </c>
-      <c r="K42" s="25" t="s">
+      <c r="K42" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1760,7 +1784,7 @@
       <c r="J43">
         <v>0</v>
       </c>
-      <c r="K43" s="25" t="s">
+      <c r="K43" s="20" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1792,7 +1816,7 @@
       <c r="J44">
         <v>0</v>
       </c>
-      <c r="K44" s="19" t="s">
+      <c r="K44" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1821,20 +1845,20 @@
       <c r="J45">
         <v>0</v>
       </c>
-      <c r="K45" s="25" t="s">
+      <c r="K45" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -1842,31 +1866,31 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="14">
-        <v>0</v>
-      </c>
-      <c r="D56" s="13">
-        <v>0</v>
-      </c>
-      <c r="E56" s="3">
-        <v>0</v>
-      </c>
-      <c r="F56" s="3">
-        <v>0</v>
-      </c>
-      <c r="G56" s="3">
-        <v>0</v>
-      </c>
-      <c r="H56" s="3">
-        <v>0</v>
-      </c>
-      <c r="I56" s="3">
-        <v>0</v>
-      </c>
-      <c r="J56" s="14">
+      <c r="C56" s="10">
+        <v>0</v>
+      </c>
+      <c r="D56" s="9">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0</v>
+      </c>
+      <c r="J56" s="10">
         <v>0</v>
       </c>
       <c r="K56" t="s">
@@ -1877,137 +1901,137 @@
       <c r="A57" t="s">
         <v>25</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="14">
-        <v>1</v>
-      </c>
-      <c r="D57" s="13">
-        <v>0</v>
-      </c>
-      <c r="E57" s="3">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3">
-        <v>1</v>
-      </c>
-      <c r="G57" s="3">
-        <v>0</v>
-      </c>
-      <c r="H57" s="3">
-        <v>0</v>
-      </c>
-      <c r="I57" s="3">
-        <v>0</v>
-      </c>
-      <c r="J57" s="6">
-        <v>0</v>
-      </c>
-      <c r="K57" s="20" t="s">
+      <c r="B57" s="26"/>
+      <c r="C57" s="10">
+        <v>1</v>
+      </c>
+      <c r="D57" s="9">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
+      <c r="J57" s="4">
+        <v>0</v>
+      </c>
+      <c r="K57" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="7"/>
-      <c r="C58" s="15">
-        <v>1</v>
-      </c>
-      <c r="D58" s="13">
-        <v>0</v>
-      </c>
-      <c r="E58" s="3">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3">
-        <v>1</v>
-      </c>
-      <c r="G58" s="3">
-        <v>0</v>
-      </c>
-      <c r="H58" s="3">
-        <v>0</v>
-      </c>
-      <c r="I58" s="3">
-        <v>0</v>
-      </c>
-      <c r="J58" s="6">
-        <v>0</v>
-      </c>
-      <c r="K58" s="21" t="s">
+      <c r="A58" s="5"/>
+      <c r="C58" s="11">
+        <v>1</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0</v>
+      </c>
+      <c r="J58" s="4">
+        <v>0</v>
+      </c>
+      <c r="K58" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C59" s="14">
-        <v>1</v>
-      </c>
-      <c r="D59" s="13">
-        <v>1</v>
-      </c>
-      <c r="E59" s="3">
-        <v>0</v>
-      </c>
-      <c r="F59" s="3">
-        <v>0</v>
-      </c>
-      <c r="G59" s="3">
-        <v>1</v>
-      </c>
-      <c r="H59" s="3">
-        <v>0</v>
-      </c>
-      <c r="I59" s="3">
-        <v>0</v>
-      </c>
-      <c r="J59" s="6">
-        <v>0</v>
-      </c>
-      <c r="K59" s="21" t="s">
+      <c r="C59" s="10">
+        <v>1</v>
+      </c>
+      <c r="D59" s="9">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>0</v>
+      </c>
+      <c r="K59" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B60" s="27"/>
-      <c r="C60" s="4" t="s">
+      <c r="B60" s="22"/>
+      <c r="C60" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="24"/>
-      <c r="K60" s="20"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="16"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C61" s="14">
-        <v>1</v>
-      </c>
-      <c r="D61" s="13">
-        <v>1</v>
-      </c>
-      <c r="E61" s="3">
-        <v>1</v>
-      </c>
-      <c r="F61" s="3">
-        <v>0</v>
-      </c>
-      <c r="G61" s="3">
-        <v>0</v>
-      </c>
-      <c r="H61" s="3">
-        <v>1</v>
-      </c>
-      <c r="I61" s="3">
-        <v>0</v>
-      </c>
-      <c r="J61" s="6">
-        <v>0</v>
-      </c>
-      <c r="K61" s="22" t="s">
+      <c r="C61" s="10">
+        <v>1</v>
+      </c>
+      <c r="D61" s="9">
+        <v>1</v>
+      </c>
+      <c r="E61" s="2">
+        <v>1</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0</v>
+      </c>
+      <c r="H61" s="2">
+        <v>1</v>
+      </c>
+      <c r="I61" s="2">
+        <v>0</v>
+      </c>
+      <c r="J61" s="4">
+        <v>0</v>
+      </c>
+      <c r="K61" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2015,46 +2039,46 @@
       <c r="A62" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="24"/>
-      <c r="K62" s="20"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="29"/>
+      <c r="K62" s="16"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="7"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="14">
-        <v>1</v>
-      </c>
-      <c r="D63" s="13">
-        <v>1</v>
-      </c>
-      <c r="E63" s="3">
-        <v>1</v>
-      </c>
-      <c r="F63" s="3">
-        <v>1</v>
-      </c>
-      <c r="G63" s="3">
-        <v>0</v>
-      </c>
-      <c r="H63" s="3">
-        <v>0</v>
-      </c>
-      <c r="I63" s="3">
-        <v>1</v>
-      </c>
-      <c r="J63" s="6">
-        <v>0</v>
-      </c>
-      <c r="K63" s="22" t="s">
+      <c r="A63" s="5"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="10">
+        <v>1</v>
+      </c>
+      <c r="D63" s="9">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
+      <c r="J63" s="4">
+        <v>0</v>
+      </c>
+      <c r="K63" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2062,61 +2086,351 @@
       <c r="A64" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="29"/>
-      <c r="C64" s="4" t="s">
+      <c r="B64" s="24"/>
+      <c r="C64" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="24"/>
-      <c r="K64" s="20"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="16"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="7"/>
-      <c r="C65" s="14">
-        <v>1</v>
-      </c>
-      <c r="D65" s="13">
-        <v>1</v>
-      </c>
-      <c r="E65" s="3">
-        <v>1</v>
-      </c>
-      <c r="F65" s="3">
-        <v>1</v>
-      </c>
-      <c r="G65" s="3">
-        <v>0</v>
-      </c>
-      <c r="H65" s="3">
-        <v>0</v>
-      </c>
-      <c r="I65" s="3">
-        <v>1</v>
-      </c>
-      <c r="J65" s="6">
-        <v>0</v>
-      </c>
-      <c r="K65" s="22"/>
+      <c r="A65" s="5"/>
+      <c r="C65" s="10">
+        <v>1</v>
+      </c>
+      <c r="D65" s="9">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0</v>
+      </c>
+      <c r="I65" s="2">
+        <v>1</v>
+      </c>
+      <c r="J65" s="4">
+        <v>0</v>
+      </c>
+      <c r="K65" s="18"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C75" s="2">
+        <v>0</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2">
+        <v>0</v>
+      </c>
+      <c r="G75" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C76" s="2">
+        <v>0</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2">
+        <v>1</v>
+      </c>
+      <c r="G76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C77" s="2">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0</v>
+      </c>
+      <c r="G77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C78" s="2">
+        <v>0</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1</v>
+      </c>
+      <c r="F78" s="2">
+        <v>1</v>
+      </c>
+      <c r="G78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C79" s="2">
+        <v>0</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2">
+        <v>0</v>
+      </c>
+      <c r="G79" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C80" s="2">
+        <v>0</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2">
+        <v>1</v>
+      </c>
+      <c r="G80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C81" s="2">
+        <v>0</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2">
+        <v>1</v>
+      </c>
+      <c r="F81" s="2">
+        <v>0</v>
+      </c>
+      <c r="G81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C82" s="2">
+        <v>0</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1</v>
+      </c>
+      <c r="G82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C83" s="2">
+        <v>1</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2">
+        <v>0</v>
+      </c>
+      <c r="G83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C84" s="2">
+        <v>1</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1</v>
+      </c>
+      <c r="G84" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C85" s="2">
+        <v>1</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2">
+        <v>0</v>
+      </c>
+      <c r="G85" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C86" s="2">
+        <v>1</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1</v>
+      </c>
+      <c r="G86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C87" s="2">
+        <v>1</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2">
+        <v>0</v>
+      </c>
+      <c r="G87" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C88" s="2">
+        <v>1</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1</v>
+      </c>
+      <c r="G88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C89" s="2">
+        <v>1</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+      <c r="F89" s="2">
+        <v>0</v>
+      </c>
+      <c r="G89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C90" s="2">
+        <v>1</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1</v>
+      </c>
+      <c r="G90" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C62:J62"/>
-    <mergeCell ref="C60:J60"/>
-    <mergeCell ref="C64:J64"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C22:J22"/>
     <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C62:J62"/>
+    <mergeCell ref="C60:J60"/>
+    <mergeCell ref="C64:J64"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>